<commit_message>
Version 5.0 de Recetas+
</commit_message>
<xml_diff>
--- a/Casos de prueba-Mi_Recetario.xlsx
+++ b/Casos de prueba-Mi_Recetario.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CoderHouse - Phyton\A Recetario\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CoderHouse - Phyton\Clase 00 Trabajo Final\Llamosas-David-47765\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50E5B41-F94F-4509-A4A7-D9D271920F6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB8760A-D0DA-4CF5-8055-B336BB828551}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -82,9 +82,6 @@
     <t>Caso #5</t>
   </si>
   <si>
-    <t>Recetas+</t>
-  </si>
-  <si>
     <t>David Llamosas A.</t>
   </si>
   <si>
@@ -154,18 +151,28 @@
     <t>Deberia de actualizar los datos.</t>
   </si>
   <si>
-    <t>Aun no se cual es el error.</t>
+    <t>Ya funciona</t>
+  </si>
+  <si>
+    <t>Recetas+ V5.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -314,42 +321,42 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -364,28 +371,31 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -430,7 +440,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -793,7 +803,7 @@
                   <a14:compatExt spid="_x0000_s1030"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -839,14 +849,19 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>6</xdr:col>
           <xdr:colOff>274320</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>76200</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="571500" cy="213360"/>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>68580</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>289560</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1032" name="Check Box 8" hidden="1">
@@ -855,7 +870,7 @@
                   <a14:compatExt spid="_x0000_s1032"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18BC8B65-4173-4CAF-991F-65BE2FE1476D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -895,7 +910,7 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -1103,7 +1118,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1123,19 +1138,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E1" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>22</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
@@ -1155,7 +1170,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>5</v>
@@ -1169,19 +1184,19 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
@@ -1218,16 +1233,16 @@
         <v>15</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="16">
         <v>45207</v>
       </c>
       <c r="E7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="22" t="s">
         <v>27</v>
-      </c>
-      <c r="F7" s="22" t="s">
-        <v>28</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="4"/>
@@ -1258,16 +1273,16 @@
         <v>16</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" s="16">
         <v>45208</v>
       </c>
       <c r="E8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="22" t="s">
         <v>29</v>
-      </c>
-      <c r="F8" s="22" t="s">
-        <v>30</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="4"/>
@@ -1298,16 +1313,16 @@
         <v>17</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" s="16">
         <v>45209</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="4"/>
@@ -1338,16 +1353,16 @@
         <v>18</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" s="16">
         <v>45210</v>
       </c>
       <c r="E10" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="23" t="s">
         <v>36</v>
-      </c>
-      <c r="F10" s="23" t="s">
-        <v>37</v>
       </c>
       <c r="G10" s="17"/>
     </row>
@@ -1359,16 +1374,16 @@
         <v>19</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" s="20">
         <v>45211</v>
       </c>
       <c r="E11" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="25" t="s">
         <v>39</v>
-      </c>
-      <c r="F11" s="25" t="s">
-        <v>40</v>
       </c>
       <c r="G11" s="17"/>
     </row>
@@ -1377,19 +1392,19 @@
         <v>6</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="26" t="s">
         <v>41</v>
-      </c>
-      <c r="C12" s="26" t="s">
-        <v>42</v>
       </c>
       <c r="D12" s="27">
         <v>45211</v>
       </c>
       <c r="E12" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="29" t="s">
         <v>43</v>
-      </c>
-      <c r="F12" s="25" t="s">
-        <v>44</v>
       </c>
       <c r="G12" s="17"/>
     </row>
@@ -2374,7 +2389,7 @@
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <drawing r:id="rId1"/>

</xml_diff>